<commit_message>
Switch to enamel wire for power sense toroid on N2ADR filter board
</commit_message>
<xml_diff>
--- a/hardware/companions/releases/n2adr_e5b8/bom.assembly.xlsx
+++ b/hardware/companions/releases/n2adr_e5b8/bom.assembly.xlsx
@@ -290,10 +290,10 @@
     <t xml:space="preserve">FB1</t>
   </si>
   <si>
-    <t xml:space="preserve">21cm PFTE silver plated 24to30AWG wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400R0111-24-9</t>
+    <t xml:space="preserve">21cm Enameled Coopper Wire 24AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various</t>
   </si>
   <si>
     <t xml:space="preserve">JP1</t>
@@ -548,6 +548,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -569,12 +570,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -619,7 +622,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -630,6 +633,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -644,7 +651,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -667,25 +674,25 @@
   </sheetPr>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J:J"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="56.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="50.0663265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="50.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.41836734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="55.4438775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.1632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="48.8928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,12 +720,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -727,16 +734,16 @@
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G2" s="0" t="n">
@@ -765,7 +772,7 @@
       <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -774,7 +781,7 @@
       <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -803,7 +810,7 @@
       <c r="B4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -812,7 +819,7 @@
       <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G4" s="0" t="n">
@@ -841,7 +848,7 @@
       <c r="B5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -850,7 +857,7 @@
       <c r="E5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -879,7 +886,7 @@
       <c r="B6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -888,7 +895,7 @@
       <c r="E6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G6" s="0" t="n">
@@ -921,7 +928,7 @@
       <c r="B7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -930,7 +937,7 @@
       <c r="E7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -959,7 +966,7 @@
       <c r="B8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -968,7 +975,7 @@
       <c r="E8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -997,7 +1004,7 @@
       <c r="B9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1006,7 +1013,7 @@
       <c r="E9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G9" s="0" t="n">
@@ -1039,7 +1046,7 @@
       <c r="B10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -1048,7 +1055,7 @@
       <c r="E10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G10" s="0" t="n">
@@ -1077,7 +1084,7 @@
       <c r="B11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -1086,7 +1093,7 @@
       <c r="E11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -1111,7 +1118,7 @@
       <c r="B12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1120,7 +1127,7 @@
       <c r="E12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G12" s="0" t="n">
@@ -1149,7 +1156,7 @@
       <c r="B13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -1158,7 +1165,7 @@
       <c r="E13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G13" s="0" t="n">
@@ -1187,7 +1194,7 @@
       <c r="B14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -1196,7 +1203,7 @@
       <c r="E14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="G14" s="0" t="n">
@@ -1225,7 +1232,7 @@
       <c r="B15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -1234,7 +1241,7 @@
       <c r="E15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G15" s="0" t="n">
@@ -1263,7 +1270,7 @@
       <c r="B16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="0" t="s">
@@ -1272,7 +1279,7 @@
       <c r="E16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G16" s="0" t="n">
@@ -1310,7 +1317,7 @@
       <c r="E17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="0" t="n">
@@ -1344,7 +1351,7 @@
       <c r="E18" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G18" s="0" t="n">
@@ -1374,7 +1381,7 @@
       <c r="E19" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G19" s="0" t="n">
@@ -1399,7 +1406,7 @@
       <c r="B20" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D20" s="0" t="s">
@@ -1408,7 +1415,7 @@
       <c r="E20" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>69</v>
       </c>
       <c r="G20" s="0" t="n">
@@ -1442,7 +1449,7 @@
       <c r="E21" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G21" s="0" t="n">
@@ -1463,7 +1470,7 @@
       <c r="B22" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D22" s="0" t="s">
@@ -1472,7 +1479,7 @@
       <c r="E22" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G22" s="0" t="n">
@@ -1506,7 +1513,7 @@
       <c r="E23" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G23" s="0" t="n">
@@ -1516,12 +1523,8 @@
         <v>1</v>
       </c>
       <c r="I23" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG</v>
-      </c>
-      <c r="J23" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=400R0111-24-9")</f>
-        <v>http://www.octopart.com/search?q=400R0111-24-9</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=Magnet Wire 0.5mm Enameled Copper Wire")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=Magnet Wire 0.5mm Enameled Copper Wire</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,16 +1534,16 @@
       <c r="B24" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="0" t="n">
@@ -1578,7 +1581,7 @@
       <c r="E25" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="5" t="n">
         <v>1812</v>
       </c>
       <c r="G25" s="0" t="n">
@@ -1599,7 +1602,7 @@
       <c r="B26" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="4" t="n">
+      <c r="C26" s="5" t="n">
         <v>5977000211</v>
       </c>
       <c r="D26" s="0" t="s">
@@ -1608,7 +1611,7 @@
       <c r="E26" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G26" s="0" t="n">
@@ -1629,7 +1632,7 @@
       <c r="B27" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="0" t="s">
@@ -1638,7 +1641,7 @@
       <c r="E27" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G27" s="0" t="n">
@@ -1659,7 +1662,7 @@
       <c r="B28" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="4" t="n">
+      <c r="C28" s="5" t="n">
         <v>7447669039</v>
       </c>
       <c r="D28" s="0" t="s">
@@ -1668,7 +1671,7 @@
       <c r="E28" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="5" t="n">
         <v>1812</v>
       </c>
       <c r="G28" s="0" t="n">
@@ -1698,7 +1701,7 @@
       <c r="E29" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <v>1210</v>
       </c>
       <c r="G29" s="0" t="n">
@@ -1728,7 +1731,7 @@
       <c r="E30" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="5" t="n">
         <v>1812</v>
       </c>
       <c r="G30" s="0" t="n">
@@ -1758,7 +1761,7 @@
       <c r="E31" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="5" t="n">
         <v>1210</v>
       </c>
       <c r="G31" s="0" t="n">
@@ -1788,7 +1791,7 @@
       <c r="E32" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="5" t="n">
         <v>1210</v>
       </c>
       <c r="G32" s="0" t="n">
@@ -1818,7 +1821,7 @@
       <c r="E33" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="5" t="n">
         <v>1210</v>
       </c>
       <c r="G33" s="0" t="n">
@@ -1848,7 +1851,7 @@
       <c r="E34" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="5" t="n">
         <v>1210</v>
       </c>
       <c r="G34" s="0" t="n">
@@ -1869,7 +1872,7 @@
       <c r="B35" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D35" s="0" t="s">
@@ -1878,7 +1881,7 @@
       <c r="E35" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G35" s="0" t="n">
@@ -1903,7 +1906,7 @@
       <c r="B36" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -1912,7 +1915,7 @@
       <c r="E36" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G36" s="0" t="n">
@@ -1937,7 +1940,7 @@
       <c r="B37" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D37" s="0" t="s">
@@ -1946,7 +1949,7 @@
       <c r="E37" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G37" s="0" t="n">
@@ -1975,7 +1978,7 @@
       <c r="B38" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D38" s="0" t="s">
@@ -1984,7 +1987,7 @@
       <c r="E38" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G38" s="0" t="n">
@@ -2013,7 +2016,7 @@
       <c r="B39" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>123</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -2022,7 +2025,7 @@
       <c r="E39" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G39" s="0" t="n">
@@ -2047,7 +2050,7 @@
       <c r="B40" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D40" s="0" t="s">
@@ -2056,7 +2059,7 @@
       <c r="E40" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G40" s="0" t="n">
@@ -2081,7 +2084,7 @@
       <c r="B41" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>129</v>
       </c>
       <c r="D41" s="0" t="s">
@@ -2090,7 +2093,7 @@
       <c r="E41" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="F41" s="5" t="n">
         <v>805</v>
       </c>
       <c r="G41" s="0" t="n">
@@ -2128,7 +2131,7 @@
       <c r="E42" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="5" t="s">
         <v>134</v>
       </c>
       <c r="G42" s="0" t="n">
@@ -2158,7 +2161,7 @@
       <c r="E43" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="5" t="s">
         <v>138</v>
       </c>
       <c r="G43" s="0" t="n">
@@ -2188,7 +2191,7 @@
       <c r="E44" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="5" t="s">
         <v>142</v>
       </c>
       <c r="G44" s="0" t="n">
@@ -2218,7 +2221,7 @@
       <c r="E45" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="5" t="s">
         <v>146</v>
       </c>
       <c r="G45" s="0" t="n">
@@ -2233,69 +2236,69 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="4"/>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="6" t="s">
         <v>148</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F47" s="4"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="6" t="s">
         <v>150</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="F48" s="4"/>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>207</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="F49" s="4"/>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F50" s="4"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="F51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="F52" s="4"/>
+      <c r="B52" s="7"/>
+      <c r="F52" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>